<commit_message>
novas traducoes e melhorias
</commit_message>
<xml_diff>
--- a/Traduzido/PTBR/Lang/PTBR/Game/Area.xlsx
+++ b/Traduzido/PTBR/Lang/PTBR/Game/Area.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isy\Documents\GitHub\elin-portugues-brasileiro\Traduzido\PTBR\Lang\PTBR\Game\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Elin\Package\PTBR\Lang\PTBR\Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727EE4F2-D0A7-40AE-894E-70ADE2DEAB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995F838C-6096-4C8B-85D1-68DCF283BB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="23925" windowHeight="13755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="1" r:id="rId1"/>
@@ -214,9 +214,6 @@
     <t>Ponto de Coleta</t>
   </si>
   <si>
-    <t>Cadeia</t>
-  </si>
-  <si>
     <t>Banho Público</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t>Local para criar animais de fazenda</t>
+  </si>
+  <si>
+    <t>Prisão</t>
   </si>
 </sst>
 </file>
@@ -626,12 +626,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="16" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="16" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="35.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="16" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="25" bestFit="1" customWidth="1" collapsed="1"/>
@@ -690,13 +692,13 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s">
         <v>14</v>
@@ -722,13 +724,13 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H4" t="s">
         <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J4" t="s">
         <v>14</v>
@@ -754,7 +756,7 @@
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
@@ -814,7 +816,7 @@
         <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H8" t="s">
         <v>30</v>
@@ -837,13 +839,13 @@
         <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H9" t="s">
         <v>33</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J9" t="s">
         <v>34</v>
@@ -877,7 +879,7 @@
         <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
         <v>40</v>
@@ -886,7 +888,7 @@
         <v>41</v>
       </c>
       <c r="I11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J11" t="s">
         <v>42</v>
@@ -903,7 +905,7 @@
         <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
         <v>45</v>
@@ -920,7 +922,7 @@
         <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
@@ -937,7 +939,7 @@
         <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
         <v>51</v>

</xml_diff>